<commit_message>
Masters added for  Feature with postman api url & body data
</commit_message>
<xml_diff>
--- a/CTAWebAPI/API Calls/APICallsMalay.xlsx
+++ b/CTAWebAPI/API Calls/APICallsMalay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malay.Doshi\source\repos\CTARepo\CTAWebAPI\API Calls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97249CD-F20B-470C-93B2-62E8048F0750}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9C3A55-FC94-4D98-AF41-9719DD041D19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98A7788A-32B8-42AA-B647-165CAF1FF6BE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
   <si>
     <t>tblactionlogger</t>
   </si>
@@ -169,6 +169,30 @@
   </si>
   <si>
     <t>{"Id":156435,"_id":0,"sGBID":"123456789","nAuthRegionID":1,"sFirstName":"Malay","sSecondName":"sadsada","sFamilyName":"dasdas","sGender":"dasdas","dtDOB":"2020-09-23T00:00:00","sDOBApprox":"sdaasdasdas","sBirthPlace":"dasdasdsad","sBirthCountryID":"sadasdasdsaa","sOriginVillage":"dsadadadad","sOriginProvinceID":"sadasdsadas","sMarried":"asdasdadad","sOtherDocuments":"dsadadadada","sResidenceNumber":"asddasdasdasdasdas","sQualificationID":"dsdasdasdasd","sOccupationID":"dsadasdasas","sAliasName":"dsadasdasdasdas","sOldGreenBKNo":"asdasdasdasdas","sFstGreenBkNo":"dasdasdasdasdas","dtFormDate":"2020-09-30T00:00:00","sFathersName":"dasdsad","sFathersID":"asdasdas","sFathersGBID":"dasdasd","sMothersName":"dasdas","sMothersID":"dasdasdas","sMothersGBID":"asdasdasdas","sSpouseName":"sdasdasd","sSpouseID":"asdasdasdasd","sSpouseGBID":"sadasdasdas","nChildrenM":2,"nChildrenF":2,"sAddress1":"dasdasdasdas","sAddress2":"dasdasdasdasd","sCity":"dasdasdasdasd","sState":"asdasdsadas","sPCode":"sdasdasdaad","sCountryID":"dasdsadasdsa","sEmail":"asdasdQ@sadas.com","sPhone":"123456789","sFax":"asdasdsa","dtDeceased":"2020-09-30T00:00:00","sBookIssued":"sdaasdsa","dtValidityDate":"2020-12-24T00:00:00","sEnteredDateTime":"dasdasdasdasdas","sPaidUntil":"s2222","tibetanName":"asqwe2q3w343","tbuPlaceOfBirth":"r43534534","tbuOriginVillage":"43534534rwe342","tbuFathersName":"45345ed43","tbuMothersName":"43534wd43","tbuSpouseName":"34sd34wd342","nEnteredBy":1,"nUpdatedBy":1}</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/Feature/GetFeatures</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/Feature/GetFeature/Id=1</t>
+  </si>
+  <si>
+    <t>{"sFeature":"TestPage","nEnteredBy":0,"nUpdatedBy":0}</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/Feature/AddFeature</t>
+  </si>
+  <si>
+    <t>{"id":24,"sFeature":"Payments","nEnteredBy":0,"nUpdatedBy":0}</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/Feature/EditFeature/Id=24</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/Feature/DeleteFeature</t>
+  </si>
+  <si>
+    <t>lstfeature</t>
   </si>
 </sst>
 </file>
@@ -219,10 +243,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,11 +565,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2973F2D4-BDCD-4BA7-950A-3A406EEC5CBB}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="A2:E7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,6 +1048,81 @@
         <v>20</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>100</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>100</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>100</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>100</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>100</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D27" r:id="rId1" xr:uid="{06C65C92-BCE3-4482-BC12-EC39738C1DCC}"/>

</xml_diff>

<commit_message>
Feature user rights baseclass, repo, controller created API testing done results in excel file
</commit_message>
<xml_diff>
--- a/CTAWebAPI/API Calls/APICallsMalay.xlsx
+++ b/CTAWebAPI/API Calls/APICallsMalay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malay.Doshi\source\repos\CTARepo\CTAWebAPI\API Calls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9C3A55-FC94-4D98-AF41-9719DD041D19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC247ECE-3AD3-4CFD-B3A7-AA91C793CE85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98A7788A-32B8-42AA-B647-165CAF1FF6BE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="62">
   <si>
     <t>tblactionlogger</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>lstfeature</t>
+  </si>
+  <si>
+    <t>lnkfeatureuserrights</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/FeatureUserrights/GetFeatureUserrights</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/FeatureUserrights/GetFeatureUserrightById/Id=1</t>
+  </si>
+  <si>
+    <t>{"nFeatureID":24,"nUserRightsID":5,"nRights":0,"dtEntered":"2020-09-29T13:39:19","nEnteredBy":1}</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/FeatureUserrights/AddFeatureUserright</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/FeatureUserrights/EditFeatureUserright/Id=117</t>
+  </si>
+  <si>
+    <t>{"Id:"117,"nFeatureID":24,"nUserRightsID":5,"nRights":1,"dtEntered":"2020-09-29T13:39:19","nEnteredBy":1}</t>
+  </si>
+  <si>
+    <t>http://localhost:52013/api/FeatureUserrights/DeleteFeatureUserright</t>
   </si>
 </sst>
 </file>
@@ -565,11 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2973F2D4-BDCD-4BA7-950A-3A406EEC5CBB}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +601,7 @@
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1109,7 +1133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>9</v>
       </c>
@@ -1121,14 +1145,91 @@
       </c>
       <c r="E49" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>100</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>100</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>100</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>100</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>100</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D27" r:id="rId1" xr:uid="{06C65C92-BCE3-4482-BC12-EC39738C1DCC}"/>
     <hyperlink ref="D28" r:id="rId2" xr:uid="{A91FD4F9-06CB-4E60-B829-A36746CBAB2F}"/>
+    <hyperlink ref="D54" r:id="rId3" xr:uid="{02506A78-6119-4F7A-AF65-2AA0DA7E93F9}"/>
+    <hyperlink ref="D56" r:id="rId4" xr:uid="{5A39E4F3-E652-45AA-B539-CF3DD7242439}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>